<commit_message>
add perancnagan pengujian done, bab 4 done inshaallah
</commit_message>
<xml_diff>
--- a/Code/skripsi.xlsx
+++ b/Code/skripsi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radityarin/Documents/Kuliah/Skripsi/Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A803063-AD2C-A54F-962E-5626D0C2CDE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA9C5CE-B143-AD4A-870A-52B4B5FC138A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{3413B29C-560F-AE4D-9915-B4DC0247194E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="6" xr2:uid="{3413B29C-560F-AE4D-9915-B4DC0247194E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Utama Pilihan" sheetId="2" r:id="rId1"/>
@@ -5060,18 +5060,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5093,6 +5081,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5105,65 +5096,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5214,6 +5157,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5561,7 +5561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D895E53-141D-0E4E-8B10-C16E118F9F44}">
   <dimension ref="A1:I390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="119" workbookViewId="0">
+    <sheetView topLeftCell="B8" zoomScale="119" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -24676,24 +24676,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="91" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="G1" s="102" t="s">
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="G1" s="99" t="s">
         <v>313</v>
       </c>
-      <c r="H1" s="102"/>
+      <c r="H1" s="99"/>
     </row>
     <row r="2" spans="2:18" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
       <c r="K2" s="24"/>
@@ -24718,16 +24718,16 @@
       <c r="E3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="102" t="s">
         <v>376</v>
       </c>
-      <c r="H3" s="105"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
-      <c r="K3" s="91" t="s">
+      <c r="K3" s="103" t="s">
         <v>320</v>
       </c>
-      <c r="L3" s="91"/>
+      <c r="L3" s="103"/>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
@@ -24750,8 +24750,8 @@
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
+      <c r="K4" s="103"/>
+      <c r="L4" s="103"/>
       <c r="M4" s="25"/>
       <c r="N4" s="25"/>
       <c r="O4" s="25"/>
@@ -24771,10 +24771,10 @@
       <c r="E5" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="100" t="s">
         <v>375</v>
       </c>
-      <c r="H5" s="104"/>
+      <c r="H5" s="101"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
       <c r="K5" s="20" t="s">
@@ -24802,7 +24802,7 @@
       <c r="E6" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="92" t="s">
+      <c r="G6" s="104" t="s">
         <v>280</v>
       </c>
       <c r="H6" s="29" t="s">
@@ -24835,7 +24835,7 @@
       <c r="E7" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="93"/>
+      <c r="G7" s="105"/>
       <c r="H7" s="20" t="s">
         <v>292</v>
       </c>
@@ -24866,7 +24866,7 @@
       <c r="E8" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="93"/>
+      <c r="G8" s="105"/>
       <c r="H8" s="20" t="s">
         <v>293</v>
       </c>
@@ -24926,7 +24926,7 @@
       <c r="E10" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="98" t="s">
         <v>173</v>
       </c>
       <c r="H10" s="20" t="s">
@@ -24959,7 +24959,7 @@
       <c r="E11" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="G11" s="94"/>
+      <c r="G11" s="98"/>
       <c r="H11" s="20" t="s">
         <v>292</v>
       </c>
@@ -24990,7 +24990,7 @@
       <c r="E12" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="94"/>
+      <c r="G12" s="98"/>
       <c r="H12" s="20" t="s">
         <v>293</v>
       </c>
@@ -25033,7 +25033,7 @@
       <c r="E14" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="G14" s="94" t="s">
+      <c r="G14" s="98" t="s">
         <v>110</v>
       </c>
       <c r="H14" s="20" t="s">
@@ -25057,7 +25057,7 @@
       <c r="C15" s="82"/>
       <c r="D15" s="82"/>
       <c r="E15" s="83"/>
-      <c r="G15" s="94"/>
+      <c r="G15" s="98"/>
       <c r="H15" s="20" t="s">
         <v>294</v>
       </c>
@@ -25079,7 +25079,7 @@
       <c r="C16" s="82"/>
       <c r="D16" s="82"/>
       <c r="E16" s="83"/>
-      <c r="G16" s="94"/>
+      <c r="G16" s="98"/>
       <c r="H16" s="20" t="s">
         <v>295</v>
       </c>
@@ -25121,7 +25121,7 @@
       <c r="C18" s="82"/>
       <c r="D18" s="82"/>
       <c r="E18" s="83"/>
-      <c r="G18" s="94" t="s">
+      <c r="G18" s="98" t="s">
         <v>245</v>
       </c>
       <c r="H18" s="20" t="s">
@@ -25145,7 +25145,7 @@
       <c r="C19" s="82"/>
       <c r="D19" s="82"/>
       <c r="E19" s="83"/>
-      <c r="G19" s="94"/>
+      <c r="G19" s="98"/>
       <c r="H19" s="20" t="s">
         <v>297</v>
       </c>
@@ -25167,7 +25167,7 @@
       <c r="C20" s="82"/>
       <c r="D20" s="82"/>
       <c r="E20" s="83"/>
-      <c r="G20" s="94"/>
+      <c r="G20" s="98"/>
       <c r="H20" s="20" t="s">
         <v>298</v>
       </c>
@@ -25203,7 +25203,7 @@
       <c r="Q21" s="25"/>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G22" s="94" t="s">
+      <c r="G22" s="98" t="s">
         <v>124</v>
       </c>
       <c r="H22" s="20" t="s">
@@ -25224,7 +25224,7 @@
       <c r="Q22" s="25"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G23" s="94"/>
+      <c r="G23" s="98"/>
       <c r="H23" s="20" t="s">
         <v>299</v>
       </c>
@@ -25243,7 +25243,7 @@
       <c r="Q23" s="25"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G24" s="94"/>
+      <c r="G24" s="98"/>
       <c r="H24" s="20" t="s">
         <v>300</v>
       </c>
@@ -25279,7 +25279,7 @@
       <c r="Q25" s="25"/>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G26" s="94" t="s">
+      <c r="G26" s="98" t="s">
         <v>248</v>
       </c>
       <c r="H26" s="20" t="s">
@@ -25300,7 +25300,7 @@
       <c r="Q26" s="25"/>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G27" s="94"/>
+      <c r="G27" s="98"/>
       <c r="H27" s="20" t="s">
         <v>301</v>
       </c>
@@ -25319,7 +25319,7 @@
       <c r="Q27" s="25"/>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G28" s="94"/>
+      <c r="G28" s="98"/>
       <c r="H28" s="20" t="s">
         <v>302</v>
       </c>
@@ -25355,7 +25355,7 @@
       <c r="Q29" s="25"/>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G30" s="94" t="s">
+      <c r="G30" s="98" t="s">
         <v>174</v>
       </c>
       <c r="H30" s="20" t="s">
@@ -25376,7 +25376,7 @@
       <c r="Q30" s="25"/>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G31" s="94"/>
+      <c r="G31" s="98"/>
       <c r="H31" s="20" t="s">
         <v>292</v>
       </c>
@@ -25395,7 +25395,7 @@
       <c r="Q31" s="25"/>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="G32" s="94"/>
+      <c r="G32" s="98"/>
       <c r="H32" s="20" t="s">
         <v>293</v>
       </c>
@@ -25431,7 +25431,7 @@
       <c r="Q33" s="25"/>
     </row>
     <row r="34" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G34" s="94" t="s">
+      <c r="G34" s="98" t="s">
         <v>244</v>
       </c>
       <c r="H34" s="20" t="s">
@@ -25452,7 +25452,7 @@
       <c r="Q34" s="25"/>
     </row>
     <row r="35" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G35" s="94"/>
+      <c r="G35" s="98"/>
       <c r="H35" s="20" t="s">
         <v>303</v>
       </c>
@@ -25471,7 +25471,7 @@
       <c r="Q35" s="25"/>
     </row>
     <row r="36" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G36" s="94"/>
+      <c r="G36" s="98"/>
       <c r="H36" s="20" t="s">
         <v>304</v>
       </c>
@@ -25507,7 +25507,7 @@
       <c r="Q37" s="25"/>
     </row>
     <row r="38" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G38" s="94" t="s">
+      <c r="G38" s="98" t="s">
         <v>154</v>
       </c>
       <c r="H38" s="20" t="s">
@@ -25528,7 +25528,7 @@
       <c r="Q38" s="25"/>
     </row>
     <row r="39" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G39" s="94"/>
+      <c r="G39" s="98"/>
       <c r="H39" s="20" t="s">
         <v>297</v>
       </c>
@@ -25547,7 +25547,7 @@
       <c r="Q39" s="25"/>
     </row>
     <row r="40" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G40" s="94"/>
+      <c r="G40" s="98"/>
       <c r="H40" s="20" t="s">
         <v>305</v>
       </c>
@@ -25583,7 +25583,7 @@
       <c r="Q41" s="25"/>
     </row>
     <row r="42" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G42" s="94" t="s">
+      <c r="G42" s="98" t="s">
         <v>281</v>
       </c>
       <c r="H42" s="20" t="s">
@@ -25604,7 +25604,7 @@
       <c r="Q42" s="25"/>
     </row>
     <row r="43" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G43" s="94"/>
+      <c r="G43" s="98"/>
       <c r="H43" s="20" t="s">
         <v>292</v>
       </c>
@@ -25623,7 +25623,7 @@
       <c r="Q43" s="25"/>
     </row>
     <row r="44" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G44" s="94"/>
+      <c r="G44" s="98"/>
       <c r="H44" s="20" t="s">
         <v>293</v>
       </c>
@@ -25659,7 +25659,7 @@
       <c r="Q45" s="25"/>
     </row>
     <row r="46" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G46" s="94" t="s">
+      <c r="G46" s="98" t="s">
         <v>282</v>
       </c>
       <c r="H46" s="20" t="s">
@@ -25680,7 +25680,7 @@
       <c r="Q46" s="25"/>
     </row>
     <row r="47" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G47" s="94"/>
+      <c r="G47" s="98"/>
       <c r="H47" s="20" t="s">
         <v>292</v>
       </c>
@@ -25699,7 +25699,7 @@
       <c r="Q47" s="25"/>
     </row>
     <row r="48" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G48" s="94"/>
+      <c r="G48" s="98"/>
       <c r="H48" s="20" t="s">
         <v>293</v>
       </c>
@@ -25735,7 +25735,7 @@
       <c r="Q49" s="25"/>
     </row>
     <row r="50" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G50" s="94" t="s">
+      <c r="G50" s="98" t="s">
         <v>277</v>
       </c>
       <c r="H50" s="20" t="s">
@@ -25756,7 +25756,7 @@
       <c r="Q50" s="25"/>
     </row>
     <row r="51" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G51" s="94"/>
+      <c r="G51" s="98"/>
       <c r="H51" s="20" t="s">
         <v>306</v>
       </c>
@@ -25775,7 +25775,7 @@
       <c r="Q51" s="25"/>
     </row>
     <row r="52" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G52" s="94"/>
+      <c r="G52" s="98"/>
       <c r="H52" s="20" t="s">
         <v>307</v>
       </c>
@@ -25811,7 +25811,7 @@
       <c r="Q53" s="25"/>
     </row>
     <row r="54" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G54" s="94" t="s">
+      <c r="G54" s="98" t="s">
         <v>163</v>
       </c>
       <c r="H54" s="20" t="s">
@@ -25832,7 +25832,7 @@
       <c r="Q54" s="25"/>
     </row>
     <row r="55" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G55" s="94"/>
+      <c r="G55" s="98"/>
       <c r="H55" s="20" t="s">
         <v>306</v>
       </c>
@@ -25851,7 +25851,7 @@
       <c r="Q55" s="25"/>
     </row>
     <row r="56" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G56" s="94"/>
+      <c r="G56" s="98"/>
       <c r="H56" s="20" t="s">
         <v>307</v>
       </c>
@@ -25887,7 +25887,7 @@
       <c r="Q57" s="25"/>
     </row>
     <row r="58" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G58" s="94" t="s">
+      <c r="G58" s="98" t="s">
         <v>175</v>
       </c>
       <c r="H58" s="20" t="s">
@@ -25908,7 +25908,7 @@
       <c r="Q58" s="25"/>
     </row>
     <row r="59" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G59" s="94"/>
+      <c r="G59" s="98"/>
       <c r="H59" s="20" t="s">
         <v>292</v>
       </c>
@@ -25927,7 +25927,7 @@
       <c r="Q59" s="25"/>
     </row>
     <row r="60" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G60" s="94"/>
+      <c r="G60" s="98"/>
       <c r="H60" s="20" t="s">
         <v>293</v>
       </c>
@@ -25963,7 +25963,7 @@
       <c r="Q61" s="25"/>
     </row>
     <row r="62" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G62" s="94" t="s">
+      <c r="G62" s="98" t="s">
         <v>283</v>
       </c>
       <c r="H62" s="20" t="s">
@@ -25984,7 +25984,7 @@
       <c r="Q62" s="25"/>
     </row>
     <row r="63" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G63" s="94"/>
+      <c r="G63" s="98"/>
       <c r="H63" s="20" t="s">
         <v>292</v>
       </c>
@@ -26003,7 +26003,7 @@
       <c r="Q63" s="25"/>
     </row>
     <row r="64" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G64" s="94"/>
+      <c r="G64" s="98"/>
       <c r="H64" s="20" t="s">
         <v>293</v>
       </c>
@@ -26039,7 +26039,7 @@
       <c r="Q65" s="25"/>
     </row>
     <row r="66" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G66" s="94" t="s">
+      <c r="G66" s="98" t="s">
         <v>176</v>
       </c>
       <c r="H66" s="20" t="s">
@@ -26060,7 +26060,7 @@
       <c r="Q66" s="25"/>
     </row>
     <row r="67" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G67" s="94"/>
+      <c r="G67" s="98"/>
       <c r="H67" s="20" t="s">
         <v>292</v>
       </c>
@@ -26079,7 +26079,7 @@
       <c r="Q67" s="25"/>
     </row>
     <row r="68" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G68" s="94"/>
+      <c r="G68" s="98"/>
       <c r="H68" s="20" t="s">
         <v>293</v>
       </c>
@@ -26115,7 +26115,7 @@
       <c r="Q69" s="25"/>
     </row>
     <row r="70" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G70" s="94" t="s">
+      <c r="G70" s="98" t="s">
         <v>234</v>
       </c>
       <c r="H70" s="20" t="s">
@@ -26136,7 +26136,7 @@
       <c r="Q70" s="25"/>
     </row>
     <row r="71" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G71" s="94"/>
+      <c r="G71" s="98"/>
       <c r="H71" s="20" t="s">
         <v>303</v>
       </c>
@@ -26155,7 +26155,7 @@
       <c r="Q71" s="25"/>
     </row>
     <row r="72" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G72" s="94"/>
+      <c r="G72" s="98"/>
       <c r="H72" s="20" t="s">
         <v>304</v>
       </c>
@@ -26191,7 +26191,7 @@
       <c r="Q73" s="25"/>
     </row>
     <row r="74" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G74" s="94" t="s">
+      <c r="G74" s="98" t="s">
         <v>255</v>
       </c>
       <c r="H74" s="20" t="s">
@@ -26212,7 +26212,7 @@
       <c r="Q74" s="25"/>
     </row>
     <row r="75" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G75" s="94"/>
+      <c r="G75" s="98"/>
       <c r="H75" s="20" t="s">
         <v>308</v>
       </c>
@@ -26231,7 +26231,7 @@
       <c r="Q75" s="25"/>
     </row>
     <row r="76" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G76" s="94"/>
+      <c r="G76" s="98"/>
       <c r="H76" s="20" t="s">
         <v>309</v>
       </c>
@@ -26267,7 +26267,7 @@
       <c r="Q77" s="25"/>
     </row>
     <row r="78" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G78" s="94" t="s">
+      <c r="G78" s="98" t="s">
         <v>177</v>
       </c>
       <c r="H78" s="20" t="s">
@@ -26288,7 +26288,7 @@
       <c r="Q78" s="25"/>
     </row>
     <row r="79" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G79" s="94"/>
+      <c r="G79" s="98"/>
       <c r="H79" s="20" t="s">
         <v>306</v>
       </c>
@@ -26307,7 +26307,7 @@
       <c r="Q79" s="25"/>
     </row>
     <row r="80" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G80" s="94"/>
+      <c r="G80" s="98"/>
       <c r="H80" s="20" t="s">
         <v>310</v>
       </c>
@@ -26343,7 +26343,7 @@
       <c r="Q81" s="25"/>
     </row>
     <row r="82" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G82" s="94" t="s">
+      <c r="G82" s="98" t="s">
         <v>178</v>
       </c>
       <c r="H82" s="20" t="s">
@@ -26364,7 +26364,7 @@
       <c r="Q82" s="25"/>
     </row>
     <row r="83" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G83" s="94"/>
+      <c r="G83" s="98"/>
       <c r="H83" s="20" t="s">
         <v>292</v>
       </c>
@@ -26383,7 +26383,7 @@
       <c r="Q83" s="25"/>
     </row>
     <row r="84" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G84" s="94"/>
+      <c r="G84" s="98"/>
       <c r="H84" s="20" t="s">
         <v>293</v>
       </c>
@@ -26419,7 +26419,7 @@
       <c r="Q85" s="25"/>
     </row>
     <row r="86" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G86" s="94" t="s">
+      <c r="G86" s="98" t="s">
         <v>179</v>
       </c>
       <c r="H86" s="20" t="s">
@@ -26440,7 +26440,7 @@
       <c r="Q86" s="25"/>
     </row>
     <row r="87" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G87" s="94"/>
+      <c r="G87" s="98"/>
       <c r="H87" s="20" t="s">
         <v>292</v>
       </c>
@@ -26459,7 +26459,7 @@
       <c r="Q87" s="25"/>
     </row>
     <row r="88" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G88" s="94"/>
+      <c r="G88" s="98"/>
       <c r="H88" s="20" t="s">
         <v>293</v>
       </c>
@@ -26495,7 +26495,7 @@
       <c r="Q89" s="25"/>
     </row>
     <row r="90" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G90" s="94" t="s">
+      <c r="G90" s="98" t="s">
         <v>180</v>
       </c>
       <c r="H90" s="20" t="s">
@@ -26516,7 +26516,7 @@
       <c r="Q90" s="25"/>
     </row>
     <row r="91" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G91" s="94"/>
+      <c r="G91" s="98"/>
       <c r="H91" s="20" t="s">
         <v>292</v>
       </c>
@@ -26535,7 +26535,7 @@
       <c r="Q91" s="25"/>
     </row>
     <row r="92" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G92" s="94"/>
+      <c r="G92" s="98"/>
       <c r="H92" s="20" t="s">
         <v>293</v>
       </c>
@@ -26571,7 +26571,7 @@
       <c r="Q93" s="25"/>
     </row>
     <row r="94" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G94" s="94" t="s">
+      <c r="G94" s="98" t="s">
         <v>279</v>
       </c>
       <c r="H94" s="20" t="s">
@@ -26592,7 +26592,7 @@
       <c r="Q94" s="25"/>
     </row>
     <row r="95" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G95" s="94"/>
+      <c r="G95" s="98"/>
       <c r="H95" s="20" t="s">
         <v>306</v>
       </c>
@@ -26611,7 +26611,7 @@
       <c r="Q95" s="25"/>
     </row>
     <row r="96" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G96" s="94"/>
+      <c r="G96" s="98"/>
       <c r="H96" s="20" t="s">
         <v>307</v>
       </c>
@@ -26647,7 +26647,7 @@
       <c r="Q97" s="25"/>
     </row>
     <row r="98" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G98" s="94" t="s">
+      <c r="G98" s="98" t="s">
         <v>181</v>
       </c>
       <c r="H98" s="20" t="s">
@@ -26668,7 +26668,7 @@
       <c r="Q98" s="25"/>
     </row>
     <row r="99" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G99" s="94"/>
+      <c r="G99" s="98"/>
       <c r="H99" s="20" t="s">
         <v>292</v>
       </c>
@@ -26687,7 +26687,7 @@
       <c r="Q99" s="25"/>
     </row>
     <row r="100" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G100" s="94"/>
+      <c r="G100" s="98"/>
       <c r="H100" s="20" t="s">
         <v>293</v>
       </c>
@@ -26723,7 +26723,7 @@
       <c r="Q101" s="25"/>
     </row>
     <row r="102" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G102" s="94" t="s">
+      <c r="G102" s="98" t="s">
         <v>258</v>
       </c>
       <c r="H102" s="20" t="s">
@@ -26744,7 +26744,7 @@
       <c r="Q102" s="25"/>
     </row>
     <row r="103" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G103" s="94"/>
+      <c r="G103" s="98"/>
       <c r="H103" s="20" t="s">
         <v>311</v>
       </c>
@@ -26763,7 +26763,7 @@
       <c r="Q103" s="25"/>
     </row>
     <row r="104" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G104" s="94"/>
+      <c r="G104" s="98"/>
       <c r="H104" s="20" t="s">
         <v>312</v>
       </c>
@@ -26799,7 +26799,7 @@
       <c r="Q105" s="25"/>
     </row>
     <row r="106" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G106" s="94" t="s">
+      <c r="G106" s="98" t="s">
         <v>182</v>
       </c>
       <c r="H106" s="20" t="s">
@@ -26820,7 +26820,7 @@
       <c r="Q106" s="25"/>
     </row>
     <row r="107" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G107" s="94"/>
+      <c r="G107" s="98"/>
       <c r="H107" s="20" t="s">
         <v>292</v>
       </c>
@@ -26839,7 +26839,7 @@
       <c r="Q107" s="25"/>
     </row>
     <row r="108" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G108" s="94"/>
+      <c r="G108" s="98"/>
       <c r="H108" s="20" t="s">
         <v>293</v>
       </c>
@@ -26875,7 +26875,7 @@
       <c r="Q109" s="25"/>
     </row>
     <row r="110" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G110" s="94" t="s">
+      <c r="G110" s="98" t="s">
         <v>151</v>
       </c>
       <c r="H110" s="20" t="s">
@@ -26896,7 +26896,7 @@
       <c r="Q110" s="25"/>
     </row>
     <row r="111" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G111" s="94"/>
+      <c r="G111" s="98"/>
       <c r="H111" s="20" t="s">
         <v>306</v>
       </c>
@@ -26915,7 +26915,7 @@
       <c r="Q111" s="25"/>
     </row>
     <row r="112" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G112" s="94"/>
+      <c r="G112" s="98"/>
       <c r="H112" s="20" t="s">
         <v>307</v>
       </c>
@@ -26951,7 +26951,7 @@
       <c r="Q113" s="25"/>
     </row>
     <row r="114" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G114" s="94" t="s">
+      <c r="G114" s="98" t="s">
         <v>275</v>
       </c>
       <c r="H114" s="20" t="s">
@@ -26972,7 +26972,7 @@
       <c r="Q114" s="25"/>
     </row>
     <row r="115" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G115" s="94"/>
+      <c r="G115" s="98"/>
       <c r="H115" s="20" t="s">
         <v>311</v>
       </c>
@@ -26991,7 +26991,7 @@
       <c r="Q115" s="25"/>
     </row>
     <row r="116" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G116" s="94"/>
+      <c r="G116" s="98"/>
       <c r="H116" s="20" t="s">
         <v>312</v>
       </c>
@@ -27027,7 +27027,7 @@
       <c r="Q117" s="25"/>
     </row>
     <row r="118" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G118" s="94" t="s">
+      <c r="G118" s="98" t="s">
         <v>183</v>
       </c>
       <c r="H118" s="20" t="s">
@@ -27048,7 +27048,7 @@
       <c r="Q118" s="25"/>
     </row>
     <row r="119" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G119" s="94"/>
+      <c r="G119" s="98"/>
       <c r="H119" s="20" t="s">
         <v>292</v>
       </c>
@@ -27067,7 +27067,7 @@
       <c r="Q119" s="25"/>
     </row>
     <row r="120" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G120" s="94"/>
+      <c r="G120" s="98"/>
       <c r="H120" s="20" t="s">
         <v>293</v>
       </c>
@@ -27103,7 +27103,7 @@
       <c r="Q121" s="25"/>
     </row>
     <row r="122" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G122" s="94" t="s">
+      <c r="G122" s="98" t="s">
         <v>111</v>
       </c>
       <c r="H122" s="20" t="s">
@@ -27124,7 +27124,7 @@
       <c r="Q122" s="25"/>
     </row>
     <row r="123" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G123" s="94"/>
+      <c r="G123" s="98"/>
       <c r="H123" s="20" t="s">
         <v>294</v>
       </c>
@@ -27143,7 +27143,7 @@
       <c r="Q123" s="25"/>
     </row>
     <row r="124" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G124" s="94"/>
+      <c r="G124" s="98"/>
       <c r="H124" s="20" t="s">
         <v>295</v>
       </c>
@@ -27179,7 +27179,7 @@
       <c r="Q125" s="25"/>
     </row>
     <row r="126" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G126" s="94" t="s">
+      <c r="G126" s="98" t="s">
         <v>184</v>
       </c>
       <c r="H126" s="20" t="s">
@@ -27200,7 +27200,7 @@
       <c r="Q126" s="25"/>
     </row>
     <row r="127" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G127" s="94"/>
+      <c r="G127" s="98"/>
       <c r="H127" s="20" t="s">
         <v>292</v>
       </c>
@@ -27219,7 +27219,7 @@
       <c r="Q127" s="25"/>
     </row>
     <row r="128" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G128" s="94"/>
+      <c r="G128" s="98"/>
       <c r="H128" s="20" t="s">
         <v>293</v>
       </c>
@@ -27255,7 +27255,7 @@
       <c r="Q129" s="25"/>
     </row>
     <row r="130" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G130" s="94" t="s">
+      <c r="G130" s="98" t="s">
         <v>284</v>
       </c>
       <c r="H130" s="20" t="s">
@@ -27276,7 +27276,7 @@
       <c r="Q130" s="25"/>
     </row>
     <row r="131" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G131" s="94"/>
+      <c r="G131" s="98"/>
       <c r="H131" s="20" t="s">
         <v>292</v>
       </c>
@@ -27295,7 +27295,7 @@
       <c r="Q131" s="25"/>
     </row>
     <row r="132" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G132" s="94"/>
+      <c r="G132" s="98"/>
       <c r="H132" s="20" t="s">
         <v>293</v>
       </c>
@@ -27331,7 +27331,7 @@
       <c r="Q133" s="25"/>
     </row>
     <row r="134" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G134" s="94" t="s">
+      <c r="G134" s="98" t="s">
         <v>185</v>
       </c>
       <c r="H134" s="20" t="s">
@@ -27352,7 +27352,7 @@
       <c r="Q134" s="25"/>
     </row>
     <row r="135" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G135" s="94"/>
+      <c r="G135" s="98"/>
       <c r="H135" s="20" t="s">
         <v>292</v>
       </c>
@@ -27371,7 +27371,7 @@
       <c r="Q135" s="25"/>
     </row>
     <row r="136" spans="7:17" x14ac:dyDescent="0.2">
-      <c r="G136" s="94"/>
+      <c r="G136" s="98"/>
       <c r="H136" s="20" t="s">
         <v>293</v>
       </c>
@@ -27406,10 +27406,10 @@
       <c r="Q137" s="25"/>
     </row>
     <row r="138" spans="7:17" ht="21" x14ac:dyDescent="0.2">
-      <c r="G138" s="100" t="s">
+      <c r="G138" s="96" t="s">
         <v>377</v>
       </c>
-      <c r="H138" s="101"/>
+      <c r="H138" s="97"/>
       <c r="I138" s="25"/>
       <c r="J138" s="25"/>
       <c r="K138" s="20" t="s">
@@ -27425,10 +27425,10 @@
       <c r="Q138" s="25"/>
     </row>
     <row r="139" spans="7:17" ht="24" x14ac:dyDescent="0.2">
-      <c r="G139" s="98" t="s">
+      <c r="G139" s="94" t="s">
         <v>410</v>
       </c>
-      <c r="H139" s="99"/>
+      <c r="H139" s="95"/>
       <c r="I139" s="25"/>
       <c r="J139" s="25"/>
       <c r="K139" s="20" t="s">
@@ -27721,6 +27721,32 @@
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C14:D20"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="E14:E20"/>
+    <mergeCell ref="G82:G84"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="G90:G92"/>
+    <mergeCell ref="G114:G116"/>
+    <mergeCell ref="G110:G112"/>
+    <mergeCell ref="G134:G136"/>
+    <mergeCell ref="G130:G132"/>
+    <mergeCell ref="G126:G128"/>
+    <mergeCell ref="G122:G124"/>
+    <mergeCell ref="G118:G120"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="G66:G68"/>
+    <mergeCell ref="G70:G72"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="G46:G48"/>
+    <mergeCell ref="G50:G52"/>
     <mergeCell ref="B1:E2"/>
     <mergeCell ref="G139:H139"/>
     <mergeCell ref="G138:H138"/>
@@ -27737,32 +27763,6 @@
     <mergeCell ref="G22:G24"/>
     <mergeCell ref="G26:G28"/>
     <mergeCell ref="G30:G32"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="G62:G64"/>
-    <mergeCell ref="G66:G68"/>
-    <mergeCell ref="G70:G72"/>
-    <mergeCell ref="G134:G136"/>
-    <mergeCell ref="G130:G132"/>
-    <mergeCell ref="G126:G128"/>
-    <mergeCell ref="G122:G124"/>
-    <mergeCell ref="G118:G120"/>
-    <mergeCell ref="G82:G84"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="G90:G92"/>
-    <mergeCell ref="G114:G116"/>
-    <mergeCell ref="G110:G112"/>
-    <mergeCell ref="C14:D20"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="E14:E20"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27773,7 +27773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE669EB-9A75-B741-9919-5DF03557E885}">
   <dimension ref="A1:BO166"/>
   <sheetViews>
-    <sheetView topLeftCell="BG1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BD1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="BJ14" sqref="BJ14"/>
     </sheetView>
   </sheetViews>
@@ -27803,61 +27803,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="124" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="127" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="108"/>
-      <c r="I1" s="108"/>
-      <c r="J1" s="108"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="108"/>
-      <c r="N1" s="108"/>
-      <c r="O1" s="108"/>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="R1" s="108"/>
-      <c r="S1" s="108"/>
-      <c r="T1" s="108"/>
-      <c r="U1" s="108"/>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-      <c r="X1" s="108"/>
-      <c r="Y1" s="108"/>
-      <c r="Z1" s="108"/>
-      <c r="AA1" s="108"/>
-      <c r="AB1" s="108"/>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="108"/>
-      <c r="AF1" s="108"/>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="108"/>
-      <c r="AI1" s="108"/>
-      <c r="AJ1" s="108"/>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
-      <c r="AN1" s="108"/>
-      <c r="AO1" s="108"/>
-      <c r="AP1" s="108"/>
-      <c r="AQ1" s="108"/>
-      <c r="AR1" s="108"/>
-      <c r="AS1" s="108"/>
-      <c r="AT1" s="108"/>
-      <c r="AU1" s="108"/>
-      <c r="AV1" s="108"/>
-      <c r="AW1" s="108"/>
-      <c r="AX1" s="108"/>
-      <c r="AY1" s="108"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
+      <c r="AA1" s="127"/>
+      <c r="AB1" s="127"/>
+      <c r="AC1" s="127"/>
+      <c r="AD1" s="127"/>
+      <c r="AE1" s="127"/>
+      <c r="AF1" s="127"/>
+      <c r="AG1" s="127"/>
+      <c r="AH1" s="127"/>
+      <c r="AI1" s="127"/>
+      <c r="AJ1" s="127"/>
+      <c r="AK1" s="127"/>
+      <c r="AL1" s="127"/>
+      <c r="AM1" s="127"/>
+      <c r="AN1" s="127"/>
+      <c r="AO1" s="127"/>
+      <c r="AP1" s="127"/>
+      <c r="AQ1" s="127"/>
+      <c r="AR1" s="127"/>
+      <c r="AS1" s="127"/>
+      <c r="AT1" s="127"/>
+      <c r="AU1" s="127"/>
+      <c r="AV1" s="127"/>
+      <c r="AW1" s="127"/>
+      <c r="AX1" s="127"/>
+      <c r="AY1" s="127"/>
       <c r="AZ1" s="45"/>
       <c r="BA1" s="79" t="s">
         <v>432</v>
@@ -27875,57 +27875,57 @@
       <c r="BJ1" s="6"/>
     </row>
     <row r="2" spans="1:67" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
+      <c r="A2" s="125"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="G2" s="108"/>
-      <c r="H2" s="108"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="108"/>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="108"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="108"/>
-      <c r="AD2" s="108"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="108"/>
-      <c r="AG2" s="108"/>
-      <c r="AH2" s="108"/>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="108"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="108"/>
-      <c r="AM2" s="108"/>
-      <c r="AN2" s="108"/>
-      <c r="AO2" s="108"/>
-      <c r="AP2" s="108"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="108"/>
-      <c r="AS2" s="108"/>
-      <c r="AT2" s="108"/>
-      <c r="AU2" s="108"/>
-      <c r="AV2" s="108"/>
-      <c r="AW2" s="108"/>
-      <c r="AX2" s="108"/>
-      <c r="AY2" s="108"/>
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="127"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="127"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="127"/>
+      <c r="Q2" s="127"/>
+      <c r="R2" s="127"/>
+      <c r="S2" s="127"/>
+      <c r="T2" s="127"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="127"/>
+      <c r="W2" s="127"/>
+      <c r="X2" s="127"/>
+      <c r="Y2" s="127"/>
+      <c r="Z2" s="127"/>
+      <c r="AA2" s="127"/>
+      <c r="AB2" s="127"/>
+      <c r="AC2" s="127"/>
+      <c r="AD2" s="127"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="127"/>
+      <c r="AG2" s="127"/>
+      <c r="AH2" s="127"/>
+      <c r="AI2" s="127"/>
+      <c r="AJ2" s="127"/>
+      <c r="AK2" s="127"/>
+      <c r="AL2" s="127"/>
+      <c r="AM2" s="127"/>
+      <c r="AN2" s="127"/>
+      <c r="AO2" s="127"/>
+      <c r="AP2" s="127"/>
+      <c r="AQ2" s="127"/>
+      <c r="AR2" s="127"/>
+      <c r="AS2" s="127"/>
+      <c r="AT2" s="127"/>
+      <c r="AU2" s="127"/>
+      <c r="AV2" s="127"/>
+      <c r="AW2" s="127"/>
+      <c r="AX2" s="127"/>
+      <c r="AY2" s="127"/>
       <c r="AZ2" s="45"/>
       <c r="BA2" s="79"/>
       <c r="BB2" s="79"/>
@@ -27934,13 +27934,13 @@
       <c r="BE2" s="45"/>
       <c r="BF2" s="80"/>
       <c r="BG2" s="45"/>
-      <c r="BH2" s="126" t="s">
+      <c r="BH2" s="107" t="s">
         <v>599</v>
       </c>
-      <c r="BI2" s="127"/>
-      <c r="BJ2" s="127"/>
-      <c r="BK2" s="127"/>
-      <c r="BL2" s="128"/>
+      <c r="BI2" s="108"/>
+      <c r="BJ2" s="108"/>
+      <c r="BK2" s="108"/>
+      <c r="BL2" s="109"/>
     </row>
     <row r="3" spans="1:67" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -27957,59 +27957,59 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="122" t="s">
+      <c r="G3" s="126" t="s">
         <v>204</v>
       </c>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="126"/>
+      <c r="L3" s="126"/>
+      <c r="M3" s="126"/>
+      <c r="N3" s="126"/>
+      <c r="O3" s="126"/>
+      <c r="P3" s="126"/>
       <c r="Q3" s="34"/>
-      <c r="R3" s="122" t="s">
+      <c r="R3" s="126" t="s">
         <v>213</v>
       </c>
-      <c r="S3" s="122"/>
-      <c r="T3" s="122"/>
-      <c r="U3" s="122"/>
-      <c r="V3" s="122"/>
-      <c r="W3" s="122"/>
-      <c r="X3" s="122"/>
-      <c r="Y3" s="122"/>
-      <c r="Z3" s="122"/>
-      <c r="AA3" s="122"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="126"/>
+      <c r="V3" s="126"/>
+      <c r="W3" s="126"/>
+      <c r="X3" s="126"/>
+      <c r="Y3" s="126"/>
+      <c r="Z3" s="126"/>
+      <c r="AA3" s="126"/>
       <c r="AB3" s="34"/>
-      <c r="AC3" s="123" t="s">
+      <c r="AC3" s="128" t="s">
         <v>219</v>
       </c>
-      <c r="AD3" s="124"/>
-      <c r="AE3" s="124"/>
-      <c r="AF3" s="124"/>
-      <c r="AG3" s="124"/>
-      <c r="AH3" s="124"/>
-      <c r="AI3" s="124"/>
-      <c r="AJ3" s="124"/>
-      <c r="AK3" s="124"/>
-      <c r="AL3" s="124"/>
-      <c r="AM3" s="124"/>
-      <c r="AN3" s="125"/>
+      <c r="AD3" s="129"/>
+      <c r="AE3" s="129"/>
+      <c r="AF3" s="129"/>
+      <c r="AG3" s="129"/>
+      <c r="AH3" s="129"/>
+      <c r="AI3" s="129"/>
+      <c r="AJ3" s="129"/>
+      <c r="AK3" s="129"/>
+      <c r="AL3" s="129"/>
+      <c r="AM3" s="129"/>
+      <c r="AN3" s="130"/>
       <c r="AO3" s="34"/>
-      <c r="AP3" s="122" t="s">
+      <c r="AP3" s="126" t="s">
         <v>225</v>
       </c>
-      <c r="AQ3" s="122"/>
-      <c r="AR3" s="122"/>
-      <c r="AS3" s="122"/>
-      <c r="AT3" s="122"/>
-      <c r="AU3" s="122"/>
-      <c r="AV3" s="122"/>
-      <c r="AW3" s="122"/>
-      <c r="AX3" s="122"/>
-      <c r="AY3" s="122"/>
+      <c r="AQ3" s="126"/>
+      <c r="AR3" s="126"/>
+      <c r="AS3" s="126"/>
+      <c r="AT3" s="126"/>
+      <c r="AU3" s="126"/>
+      <c r="AV3" s="126"/>
+      <c r="AW3" s="126"/>
+      <c r="AX3" s="126"/>
+      <c r="AY3" s="126"/>
       <c r="AZ3" s="44"/>
       <c r="BA3" s="81" t="s">
         <v>433</v>
@@ -28020,11 +28020,11 @@
       <c r="BE3" s="44"/>
       <c r="BF3" s="59"/>
       <c r="BG3" s="44"/>
-      <c r="BH3" s="129"/>
-      <c r="BI3" s="130"/>
-      <c r="BJ3" s="130"/>
-      <c r="BK3" s="130"/>
-      <c r="BL3" s="131"/>
+      <c r="BH3" s="110"/>
+      <c r="BI3" s="111"/>
+      <c r="BJ3" s="111"/>
+      <c r="BK3" s="111"/>
+      <c r="BL3" s="112"/>
     </row>
     <row r="4" spans="1:67" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
@@ -28354,13 +28354,13 @@
         <v>441</v>
       </c>
       <c r="BG5" s="33"/>
-      <c r="BH5" s="132"/>
-      <c r="BI5" s="134" t="s">
+      <c r="BH5" s="113"/>
+      <c r="BI5" s="115" t="s">
         <v>566</v>
       </c>
-      <c r="BJ5" s="135"/>
-      <c r="BK5" s="135"/>
-      <c r="BL5" s="136"/>
+      <c r="BJ5" s="116"/>
+      <c r="BK5" s="116"/>
+      <c r="BL5" s="117"/>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
@@ -28522,11 +28522,11 @@
       <c r="BE6" s="33"/>
       <c r="BF6" s="54"/>
       <c r="BG6" s="33"/>
-      <c r="BH6" s="133"/>
-      <c r="BI6" s="137"/>
-      <c r="BJ6" s="138"/>
-      <c r="BK6" s="138"/>
-      <c r="BL6" s="139"/>
+      <c r="BH6" s="114"/>
+      <c r="BI6" s="118"/>
+      <c r="BJ6" s="119"/>
+      <c r="BK6" s="119"/>
+      <c r="BL6" s="120"/>
       <c r="BN6" s="32" t="s">
         <v>576</v>
       </c>
@@ -28694,7 +28694,7 @@
         <v>31</v>
       </c>
       <c r="BG7" s="33"/>
-      <c r="BH7" s="140" t="s">
+      <c r="BH7" s="121" t="s">
         <v>567</v>
       </c>
       <c r="BI7" s="9"/>
@@ -28876,7 +28876,7 @@
         <v>442</v>
       </c>
       <c r="BG8" s="33"/>
-      <c r="BH8" s="141"/>
+      <c r="BH8" s="122"/>
       <c r="BI8" s="68" t="s">
         <v>7</v>
       </c>
@@ -29056,7 +29056,7 @@
       <c r="BE9" s="33"/>
       <c r="BF9" s="54"/>
       <c r="BG9" s="33"/>
-      <c r="BH9" s="141"/>
+      <c r="BH9" s="122"/>
       <c r="BI9" s="67" t="s">
         <v>10</v>
       </c>
@@ -29238,7 +29238,7 @@
         <v>439</v>
       </c>
       <c r="BG10" s="33"/>
-      <c r="BH10" s="142"/>
+      <c r="BH10" s="123"/>
       <c r="BI10" s="67" t="s">
         <v>11</v>
       </c>
@@ -29584,7 +29584,7 @@
       <c r="BE12" s="33"/>
       <c r="BF12" s="54"/>
       <c r="BG12" s="33"/>
-      <c r="BH12" s="107" t="s">
+      <c r="BH12" s="142" t="s">
         <v>7</v>
       </c>
       <c r="BI12" s="51" t="s">
@@ -29754,7 +29754,7 @@
         <v>51</v>
       </c>
       <c r="BG13" s="33"/>
-      <c r="BH13" s="107"/>
+      <c r="BH13" s="142"/>
       <c r="BI13" s="65">
         <v>2</v>
       </c>
@@ -29922,7 +29922,7 @@
         <v>443</v>
       </c>
       <c r="BG14" s="33"/>
-      <c r="BH14" s="107" t="s">
+      <c r="BH14" s="142" t="s">
         <v>10</v>
       </c>
       <c r="BI14" s="69" t="s">
@@ -29939,12 +29939,12 @@
       </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="124" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="35" t="s">
@@ -30092,7 +30092,7 @@
       <c r="BE15" s="33"/>
       <c r="BF15" s="54"/>
       <c r="BG15" s="33"/>
-      <c r="BH15" s="107"/>
+      <c r="BH15" s="142"/>
       <c r="BI15" s="65">
         <v>1</v>
       </c>
@@ -30107,10 +30107,10 @@
       </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.2">
-      <c r="A16" s="119"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
+      <c r="A16" s="125"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="125"/>
+      <c r="D16" s="125"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="35" t="s">
@@ -30260,7 +30260,7 @@
         <v>440</v>
       </c>
       <c r="BG16" s="33"/>
-      <c r="BH16" s="107" t="s">
+      <c r="BH16" s="142" t="s">
         <v>11</v>
       </c>
       <c r="BI16" s="51" t="s">
@@ -30438,7 +30438,7 @@
         <v>444</v>
       </c>
       <c r="BG17" s="33"/>
-      <c r="BH17" s="107"/>
+      <c r="BH17" s="142"/>
       <c r="BI17" s="65">
         <v>1</v>
       </c>
@@ -32351,12 +32351,12 @@
       </c>
     </row>
     <row r="29" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="118"/>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="124"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="35" t="s">
@@ -32519,10 +32519,10 @@
       </c>
     </row>
     <row r="30" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A30" s="119"/>
-      <c r="B30" s="119"/>
-      <c r="C30" s="119"/>
-      <c r="D30" s="119"/>
+      <c r="A30" s="125"/>
+      <c r="B30" s="125"/>
+      <c r="C30" s="125"/>
+      <c r="D30" s="125"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="35" t="s">
@@ -34665,12 +34665,12 @@
       <c r="BJ42" s="6"/>
     </row>
     <row r="43" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A43" s="108" t="s">
+      <c r="A43" s="127" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="108"/>
-      <c r="C43" s="108"/>
-      <c r="D43" s="108"/>
+      <c r="B43" s="127"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="35" t="s">
@@ -34825,10 +34825,10 @@
       <c r="BJ43" s="6"/>
     </row>
     <row r="44" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A44" s="108"/>
-      <c r="B44" s="108"/>
-      <c r="C44" s="108"/>
-      <c r="D44" s="108"/>
+      <c r="A44" s="127"/>
+      <c r="B44" s="127"/>
+      <c r="C44" s="127"/>
+      <c r="D44" s="127"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="35" t="s">
@@ -36793,12 +36793,12 @@
       <c r="BJ55" s="6"/>
     </row>
     <row r="56" spans="1:62" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="120" t="s">
+      <c r="A56" s="140" t="s">
         <v>411</v>
       </c>
-      <c r="B56" s="120"/>
-      <c r="C56" s="120"/>
-      <c r="D56" s="120"/>
+      <c r="B56" s="140"/>
+      <c r="C56" s="140"/>
+      <c r="D56" s="140"/>
       <c r="E56" s="25"/>
       <c r="F56" s="6"/>
       <c r="G56" s="35" t="s">
@@ -36953,10 +36953,10 @@
       <c r="BJ56" s="6"/>
     </row>
     <row r="57" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A57" s="120"/>
-      <c r="B57" s="120"/>
-      <c r="C57" s="120"/>
-      <c r="D57" s="120"/>
+      <c r="A57" s="140"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="140"/>
+      <c r="D57" s="140"/>
       <c r="E57" s="25"/>
       <c r="F57" s="6"/>
       <c r="G57" s="35" t="s">
@@ -37111,12 +37111,12 @@
       <c r="BJ57" s="6"/>
     </row>
     <row r="58" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A58" s="121" t="s">
+      <c r="A58" s="141" t="s">
         <v>379</v>
       </c>
-      <c r="B58" s="121"/>
-      <c r="C58" s="121"/>
-      <c r="D58" s="121"/>
+      <c r="B58" s="141"/>
+      <c r="C58" s="141"/>
+      <c r="D58" s="141"/>
       <c r="E58" s="25"/>
       <c r="F58" s="6"/>
       <c r="G58" s="35" t="s">
@@ -37577,12 +37577,12 @@
       <c r="BJ60" s="6"/>
     </row>
     <row r="61" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A61" s="108" t="s">
+      <c r="A61" s="127" t="s">
         <v>378</v>
       </c>
-      <c r="B61" s="108"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
+      <c r="B61" s="127"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="127"/>
       <c r="E61" s="25"/>
       <c r="F61" s="6"/>
       <c r="G61" s="35" t="s">
@@ -37737,10 +37737,10 @@
       <c r="BJ61" s="6"/>
     </row>
     <row r="62" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A62" s="108"/>
-      <c r="B62" s="108"/>
-      <c r="C62" s="108"/>
-      <c r="D62" s="108"/>
+      <c r="A62" s="127"/>
+      <c r="B62" s="127"/>
+      <c r="C62" s="127"/>
+      <c r="D62" s="127"/>
       <c r="E62" s="25"/>
       <c r="F62" s="6"/>
       <c r="G62" s="35" t="s">
@@ -39863,12 +39863,12 @@
       <c r="BJ74" s="6"/>
     </row>
     <row r="75" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A75" s="108" t="s">
+      <c r="A75" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="B75" s="108"/>
-      <c r="C75" s="108"/>
-      <c r="D75" s="108"/>
+      <c r="B75" s="127"/>
+      <c r="C75" s="127"/>
+      <c r="D75" s="127"/>
       <c r="E75" s="25"/>
       <c r="F75" s="6"/>
       <c r="G75" s="35" t="s">
@@ -40021,10 +40021,10 @@
       <c r="BJ75" s="6"/>
     </row>
     <row r="76" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A76" s="108"/>
-      <c r="B76" s="108"/>
-      <c r="C76" s="108"/>
-      <c r="D76" s="108"/>
+      <c r="A76" s="127"/>
+      <c r="B76" s="127"/>
+      <c r="C76" s="127"/>
+      <c r="D76" s="127"/>
       <c r="E76" s="25"/>
       <c r="F76" s="6"/>
       <c r="G76" s="35" t="s">
@@ -42298,11 +42298,11 @@
     </row>
     <row r="90" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
-      <c r="B90" s="109" t="s">
+      <c r="B90" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="C90" s="110"/>
-      <c r="D90" s="115" t="s">
+      <c r="C90" s="132"/>
+      <c r="D90" s="137" t="s">
         <v>397</v>
       </c>
       <c r="G90" s="42" t="s">
@@ -42452,9 +42452,9 @@
     </row>
     <row r="91" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A91" s="6"/>
-      <c r="B91" s="111"/>
-      <c r="C91" s="112"/>
-      <c r="D91" s="116"/>
+      <c r="B91" s="133"/>
+      <c r="C91" s="134"/>
+      <c r="D91" s="138"/>
       <c r="G91" s="42" t="s">
         <v>282</v>
       </c>
@@ -42600,9 +42600,9 @@
     </row>
     <row r="92" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A92" s="6"/>
-      <c r="B92" s="111"/>
-      <c r="C92" s="112"/>
-      <c r="D92" s="116"/>
+      <c r="B92" s="133"/>
+      <c r="C92" s="134"/>
+      <c r="D92" s="138"/>
       <c r="G92" s="42" t="s">
         <v>175</v>
       </c>
@@ -42749,9 +42749,9 @@
       </c>
     </row>
     <row r="93" spans="1:62" ht="17" x14ac:dyDescent="0.2">
-      <c r="B93" s="111"/>
-      <c r="C93" s="112"/>
-      <c r="D93" s="116"/>
+      <c r="B93" s="133"/>
+      <c r="C93" s="134"/>
+      <c r="D93" s="138"/>
       <c r="G93" s="42" t="s">
         <v>283</v>
       </c>
@@ -42898,9 +42898,9 @@
       </c>
     </row>
     <row r="94" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="B94" s="111"/>
-      <c r="C94" s="112"/>
-      <c r="D94" s="116"/>
+      <c r="B94" s="133"/>
+      <c r="C94" s="134"/>
+      <c r="D94" s="138"/>
       <c r="G94" s="42" t="s">
         <v>176</v>
       </c>
@@ -43047,9 +43047,9 @@
       </c>
     </row>
     <row r="95" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="B95" s="111"/>
-      <c r="C95" s="112"/>
-      <c r="D95" s="116"/>
+      <c r="B95" s="133"/>
+      <c r="C95" s="134"/>
+      <c r="D95" s="138"/>
       <c r="G95" s="42" t="s">
         <v>177</v>
       </c>
@@ -43194,9 +43194,9 @@
       <c r="BF95" s="54"/>
     </row>
     <row r="96" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="B96" s="113"/>
-      <c r="C96" s="114"/>
-      <c r="D96" s="117"/>
+      <c r="B96" s="135"/>
+      <c r="C96" s="136"/>
+      <c r="D96" s="139"/>
       <c r="G96" s="42" t="s">
         <v>178</v>
       </c>
@@ -46647,30 +46647,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="BF1:BF2"/>
-    <mergeCell ref="BA1:BD2"/>
-    <mergeCell ref="BA3:BD3"/>
-    <mergeCell ref="BI29:BL29"/>
-    <mergeCell ref="BI30:BL30"/>
-    <mergeCell ref="BH2:BL3"/>
-    <mergeCell ref="BH5:BH6"/>
-    <mergeCell ref="BI5:BL6"/>
-    <mergeCell ref="BH7:BH10"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="G3:P3"/>
-    <mergeCell ref="G1:AY2"/>
-    <mergeCell ref="AP3:AY3"/>
-    <mergeCell ref="A15:D16"/>
-    <mergeCell ref="R3:AA3"/>
-    <mergeCell ref="AC3:AN3"/>
-    <mergeCell ref="A75:D76"/>
-    <mergeCell ref="B90:C96"/>
-    <mergeCell ref="D90:D96"/>
-    <mergeCell ref="A29:D30"/>
-    <mergeCell ref="A43:D44"/>
-    <mergeCell ref="A61:D62"/>
-    <mergeCell ref="A56:D57"/>
-    <mergeCell ref="A58:D58"/>
     <mergeCell ref="BI31:BL31"/>
     <mergeCell ref="BH12:BH13"/>
     <mergeCell ref="BH14:BH15"/>
@@ -46685,6 +46661,30 @@
     <mergeCell ref="BI23:BL23"/>
     <mergeCell ref="BI24:BL24"/>
     <mergeCell ref="BI25:BL25"/>
+    <mergeCell ref="A75:D76"/>
+    <mergeCell ref="B90:C96"/>
+    <mergeCell ref="D90:D96"/>
+    <mergeCell ref="A29:D30"/>
+    <mergeCell ref="A43:D44"/>
+    <mergeCell ref="A61:D62"/>
+    <mergeCell ref="A56:D57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="G3:P3"/>
+    <mergeCell ref="G1:AY2"/>
+    <mergeCell ref="AP3:AY3"/>
+    <mergeCell ref="A15:D16"/>
+    <mergeCell ref="R3:AA3"/>
+    <mergeCell ref="AC3:AN3"/>
+    <mergeCell ref="BF1:BF2"/>
+    <mergeCell ref="BA1:BD2"/>
+    <mergeCell ref="BA3:BD3"/>
+    <mergeCell ref="BI29:BL29"/>
+    <mergeCell ref="BI30:BL30"/>
+    <mergeCell ref="BH2:BL3"/>
+    <mergeCell ref="BH5:BH6"/>
+    <mergeCell ref="BI5:BL6"/>
+    <mergeCell ref="BH7:BH10"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>